<commit_message>
Rubrica 3 y video
</commit_message>
<xml_diff>
--- a/Guías/Rubricas.xlsx
+++ b/Guías/Rubricas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DATA ANALIST\Git\Proyecto Despliegue\MIAD---PROYECTO---DESPLIEGUE-DE-SOLUCIONES\Guías\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936B5672-B1B5-41DE-B2FA-E862EDB904B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D707E9A8-E322-46E0-8223-0D58DFD59D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -254,7 +254,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="[$-409]d\-mmm;@"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -272,6 +275,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -336,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -371,21 +382,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -692,11 +706,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H21" sqref="H21"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -704,13 +718,13 @@
     <col min="2" max="2" width="16.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="35.6328125" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="35.6328125" customWidth="1"/>
-    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6328125" customWidth="1"/>
+    <col min="7" max="7" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="9" t="s">
@@ -725,14 +739,14 @@
       <c r="E1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>7</v>
       </c>
@@ -753,7 +767,7 @@
       </c>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>7</v>
       </c>
@@ -774,7 +788,7 @@
       </c>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>7</v>
       </c>
@@ -795,7 +809,7 @@
       </c>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
         <v>7</v>
       </c>
@@ -816,7 +830,7 @@
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
@@ -837,7 +851,7 @@
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
         <v>7</v>
       </c>
@@ -858,7 +872,7 @@
       </c>
       <c r="G7" s="11"/>
     </row>
-    <row r="8" spans="1:7" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>36</v>
       </c>
@@ -875,13 +889,15 @@
         <v>42</v>
       </c>
       <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-    </row>
-    <row r="9" spans="1:7" ht="87" hidden="1" x14ac:dyDescent="0.35">
+      <c r="G8" s="17">
+        <v>45969</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="18" t="s">
         <v>38</v>
       </c>
       <c r="C9" s="14" t="s">
@@ -894,9 +910,11 @@
         <v>43</v>
       </c>
       <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-    </row>
-    <row r="10" spans="1:7" ht="58" hidden="1" x14ac:dyDescent="0.35">
+      <c r="G9" s="17">
+        <v>45969</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>36</v>
       </c>
@@ -913,28 +931,32 @@
         <v>44</v>
       </c>
       <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-    </row>
-    <row r="11" spans="1:7" ht="87" hidden="1" x14ac:dyDescent="0.35">
+      <c r="G10" s="17">
+        <v>45969</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="14" t="s">
         <v>54</v>
       </c>
       <c r="E11" s="16" t="s">
         <v>45</v>
       </c>
       <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-    </row>
-    <row r="12" spans="1:7" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="G11" s="17">
+        <v>45969</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
         <v>36</v>
       </c>
@@ -951,13 +973,15 @@
         <v>46</v>
       </c>
       <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
+      <c r="G12" s="17">
+        <v>45969</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G12" xr:uid="{2BD1BA79-2715-4BEA-95DC-58DC9B8F04DF}">
     <filterColumn colId="0">
       <filters>
-        <filter val="Guía 1"/>
+        <filter val="Guía 2"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>